<commit_message>
se hace mas grande el codigo de barras por que no lo alcanza a leer la pistola
se hace mas grande el codigo de barras por que no lo alcanza a leer la pistola
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99575D5-225B-4913-A404-D126A9C95606}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD1A393-8F19-4AB8-9B74-D589F7D5FA2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Observaciones</t>
   </si>
@@ -84,9 +84,6 @@
     <t xml:space="preserve">al editar no carga la clave del producto del sat </t>
   </si>
   <si>
-    <t>en ticket agrear cambios y con cuanto pago</t>
-  </si>
-  <si>
     <t>cancelaciones</t>
   </si>
   <si>
@@ -115,6 +112,15 @@
   </si>
   <si>
     <t>Monto Total de Cancelaciones</t>
+  </si>
+  <si>
+    <t>en ticket agrear cambio y con cuanto pago</t>
+  </si>
+  <si>
+    <t>APP</t>
+  </si>
+  <si>
+    <t>Alerta cuando llega un pedido y no se atendido un notificacion y ademas un campanita que tiene  un pedio por atender</t>
   </si>
 </sst>
 </file>
@@ -172,10 +178,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -490,16 +496,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2A72-8D22-4098-80BD-64C3E85E21F7}">
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="162" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -515,72 +521,72 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="3"/>
+      <c r="P2" s="4"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="3"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="4"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="4"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="4"/>
       <c r="Q6" s="2"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="4"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="4"/>
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="4"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="P10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="P10" s="4"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -589,25 +595,25 @@
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="P11" s="3"/>
+      <c r="P11" s="4"/>
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="P12" s="3"/>
+      <c r="P12" s="4"/>
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="3"/>
+      <c r="P13" s="4"/>
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P14" s="3"/>
+      <c r="P14" s="4"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -625,61 +631,71 @@
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="P19" s="4"/>
+      <c r="P19" s="3"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="P22" s="4"/>
+        <v>29</v>
+      </c>
+      <c r="P22" s="3"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" t="s">
         <v>21</v>
-      </c>
-      <c r="B24" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
se agregar codigo de barras
Se agregan codigo de barras para las busquedas en la hand held
Se actualiza la leyenda en los codigos de barras menudeo , menudeo por menudeo y mayoreo, se agrega la leyenda de super mayoreo
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD1A393-8F19-4AB8-9B74-D589F7D5FA2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3309286F-D824-4A66-A14D-3D44C043256C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Observaciones</t>
   </si>
@@ -108,9 +109,6 @@
     <t>Monto Total de Retiros</t>
   </si>
   <si>
-    <t xml:space="preserve">generar ticket si es cobro con tarje se regresa todo monto + comision </t>
-  </si>
-  <si>
     <t>Monto Total de Cancelaciones</t>
   </si>
   <si>
@@ -121,6 +119,12 @@
   </si>
   <si>
     <t>Alerta cuando llega un pedido y no se atendido un notificacion y ademas un campanita que tiene  un pedio por atender</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">generar ticket si es cobro con tarjeta se regresa todo monto + comision </t>
   </si>
 </sst>
 </file>
@@ -174,11 +178,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,13 +504,13 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -521,72 +526,72 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4"/>
+      <c r="P2" s="5"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="4"/>
+      <c r="P3" s="5"/>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="4"/>
+      <c r="P4" s="5"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="4"/>
+      <c r="P5" s="5"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="4"/>
-      <c r="Q6" s="2"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="4"/>
+      <c r="P7" s="5"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="4"/>
+      <c r="P8" s="5"/>
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="4"/>
+      <c r="P9" s="5"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="A10" s="5"/>
+      <c r="P10" s="5"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -595,25 +600,25 @@
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="P11" s="4"/>
+      <c r="P11" s="5"/>
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P12" s="4"/>
+      <c r="P12" s="5"/>
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="4"/>
+      <c r="P13" s="5"/>
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P14" s="4"/>
+      <c r="P14" s="5"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -624,7 +629,7 @@
       </c>
       <c r="Q15" s="2"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -632,70 +637,94 @@
         <v>18</v>
       </c>
       <c r="P19" s="3"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q19" s="1"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B22" t="s">
-        <v>29</v>
+      <c r="B22" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
-      <c r="B23" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="C24" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="C25" s="4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="C26" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="C29" s="4">
+        <f>C25+C26-C28</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>28</v>
+      <c r="C30" s="4">
+        <f>C29-C26-C27</f>
+        <v>1100</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -707,4 +736,136 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3A1473E-E58C-4676-9ABB-3A67EB75B525}">
+  <dimension ref="B13:Q19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>478</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>1650</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>550</v>
+      </c>
+      <c r="K13">
+        <v>467</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>550</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>41.25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <v>478</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+      <c r="H15">
+        <v>3</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>550</v>
+      </c>
+      <c r="K15">
+        <v>467</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>550</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>31</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <f>G15*0.025</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="Q16">
+        <f>Q13+Q15</f>
+        <v>66.25</v>
+      </c>
+    </row>
+    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G19">
+        <f>G13+G15</f>
+        <v>2650</v>
+      </c>
+      <c r="H19">
+        <f>G19*0.025</f>
+        <v>66.25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
vista de sesion expirada
vista de sesion expirada
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3309286F-D824-4A66-A14D-3D44C043256C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD4825A-F8E5-4716-BC08-C0500C2D26BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
@@ -178,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -187,6 +187,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,7 +505,7 @@
   <dimension ref="A1:Q34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B12" sqref="B12:Q12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,7 +527,7 @@
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="5"/>
+      <c r="P2" s="6"/>
       <c r="Q2" s="1"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -536,7 +537,7 @@
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="5"/>
+      <c r="P3" s="6"/>
       <c r="Q3" s="1"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -544,7 +545,7 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="5"/>
+      <c r="P4" s="6"/>
       <c r="Q4" s="1"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -552,7 +553,7 @@
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="5"/>
+      <c r="P5" s="6"/>
       <c r="Q5" s="1"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -560,7 +561,7 @@
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="5"/>
+      <c r="P6" s="6"/>
       <c r="Q6" s="1"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -568,7 +569,7 @@
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="5"/>
+      <c r="P7" s="6"/>
       <c r="Q7" s="2"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -578,7 +579,7 @@
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="5"/>
+      <c r="P8" s="6"/>
       <c r="Q8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -586,12 +587,12 @@
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="5"/>
+      <c r="P9" s="6"/>
       <c r="Q9" s="1"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="P10" s="5"/>
+      <c r="P10" s="6"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -600,25 +601,25 @@
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="P11" s="5"/>
+      <c r="P11" s="6"/>
       <c r="Q11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P12" s="5"/>
+      <c r="P12" s="6"/>
       <c r="Q12" s="2"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="5"/>
+      <c r="P13" s="6"/>
       <c r="Q13" s="1"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P14" s="5"/>
+      <c r="P14" s="6"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -728,11 +729,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="P2:P7"/>
-    <mergeCell ref="P8:P14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
init de tooltip en  ventas
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD4825A-F8E5-4716-BC08-C0500C2D26BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A1383C-AFDD-4B18-8D54-DB0AA9CF9091}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
+    <workbookView xWindow="13905" yWindow="2925" windowWidth="13830" windowHeight="8880" activeTab="2" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Observaciones</t>
   </si>
@@ -125,13 +126,16 @@
   </si>
   <si>
     <t xml:space="preserve">generar ticket si es cobro con tarjeta se regresa todo monto + comision </t>
+  </si>
+  <si>
+    <t>Estatus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,8 +143,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -165,6 +177,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -178,16 +196,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2A72-8D22-4098-80BD-64C3E85E21F7}">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:Q12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,216 +536,219 @@
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N1" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="N2" s="1"/>
+      <c r="P2" s="5"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
+      <c r="N3" s="1"/>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="1"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+      <c r="N4" s="1"/>
+      <c r="P4" s="5"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="1"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="N5" s="1"/>
+      <c r="P5" s="5"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="1"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="N6" s="1"/>
+      <c r="P6" s="5"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="2"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="N7" s="2"/>
+      <c r="P7" s="5"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="1"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="N8" s="1"/>
+      <c r="P8" s="5"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="1"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="P10" s="6"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N9" s="1"/>
+      <c r="P9" s="5"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="P10" s="5"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="1"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N11" s="1"/>
+      <c r="P11" s="5"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="2"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N12" s="2"/>
+      <c r="P12" s="5"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="6"/>
-      <c r="Q13" s="1"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="P14" s="6"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N13" s="1"/>
+      <c r="P13" s="5"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P14" s="5"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="Q15" s="2"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="N15" s="1"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="1"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" s="3"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>6</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P22" s="3"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>19</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B22" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="C22" s="4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="C24" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C26" s="4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C27" s="4">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <f>C23+C24-C26</f>
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C28" s="4">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C29" s="4">
-        <f>C25+C26-C28</f>
-        <v>2400</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C30" s="4">
-        <f>C29-C26-C27</f>
+        <f>C27-C24-C25</f>
         <v>1100</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>30</v>
       </c>
     </row>
@@ -867,4 +891,65 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B13416C8-9FB6-4D69-8B70-EF6AE3944725}">
+  <dimension ref="H8:I16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="8" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="9" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="10" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="11" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1223.8499999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f>SUM(H8:H11)</f>
+        <v>6558.85</v>
+      </c>
+      <c r="I12">
+        <v>977.85</v>
+      </c>
+    </row>
+    <row r="13" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <f>SUM(I12:I13)</f>
+        <v>1177.8499999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <f>H12-I14</f>
+        <v>5381</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
se acomodan nuevamente los codigos de barras
se acomodan nuevamente los codigos de barras
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F8CFA2-9EBB-47AC-911D-CA995DE3015E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B04D47-BA35-49A3-9403-41B4B59A5C48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
@@ -591,7 +591,7 @@
   <dimension ref="A1:P53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+      <selection activeCell="B32" sqref="B32:N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
aumente 3.2 cm el alto de los codigos
aumente 3.2 cm el alto de los codigos
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B04D47-BA35-49A3-9403-41B4B59A5C48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176CCE1B-DB08-452E-BC24-9CC5CD87BE41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
   <si>
     <t>Observaciones</t>
   </si>
@@ -192,6 +193,27 @@
   </si>
   <si>
     <t>Cantidad de Devoluciones por producto o por venta?</t>
+  </si>
+  <si>
+    <t>Cooperacion</t>
+  </si>
+  <si>
+    <t>TotalSesiones</t>
+  </si>
+  <si>
+    <t>Costo Por Hora</t>
+  </si>
+  <si>
+    <t>No.Horas</t>
+  </si>
+  <si>
+    <t>Costo Sesion Por Persona</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Costo Sesion Total</t>
   </si>
 </sst>
 </file>
@@ -222,7 +244,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,6 +269,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -260,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -274,6 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +617,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2A72-8D22-4098-80BD-64C3E85E21F7}">
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:N32"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,154 +630,154 @@
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="1"/>
-      <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K2" s="1"/>
+      <c r="M2" s="4"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="N3" s="1"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K3" s="1"/>
+      <c r="M3" s="4"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K4" s="1"/>
+      <c r="M4" s="4"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="1"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K5" s="1"/>
+      <c r="M5" s="4"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="8"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="1"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K6" s="1"/>
+      <c r="M6" s="4"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K7" s="2"/>
+      <c r="M7" s="4"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="N8" s="1"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K8" s="1"/>
+      <c r="M8" s="4"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="N9" s="1"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K9" s="1"/>
+      <c r="M9" s="4"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
-      <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M10" s="4"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>8</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
-      <c r="N11" s="1"/>
-      <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11" s="1"/>
+      <c r="M11" s="4"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="N12" s="7"/>
-      <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K12" s="7"/>
+      <c r="M12" s="4"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="N13" s="1"/>
-      <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K13" s="1"/>
+      <c r="M13" s="4"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M14" s="4"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="N17" s="1"/>
-      <c r="P17" s="3"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K17" s="1"/>
+      <c r="M17" s="3"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N20" s="1"/>
-      <c r="P20" s="6"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K20" s="1"/>
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N21" s="1"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -758,9 +787,9 @@
       <c r="C22" s="3">
         <v>20</v>
       </c>
-      <c r="N22" s="1"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
         <v>22</v>
       </c>
@@ -768,7 +797,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
         <v>23</v>
       </c>
@@ -776,7 +805,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
         <v>26</v>
       </c>
@@ -784,7 +813,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
         <v>27</v>
       </c>
@@ -792,7 +821,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
         <v>24</v>
       </c>
@@ -801,7 +830,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
         <v>25</v>
       </c>
@@ -810,122 +839,131 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>32</v>
       </c>
+      <c r="K31" s="1"/>
       <c r="L31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>33</v>
       </c>
+      <c r="K32" s="2"/>
       <c r="L32" t="s">
         <v>53</v>
       </c>
-      <c r="N32" s="2"/>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>34</v>
       </c>
+      <c r="K33" s="1"/>
       <c r="L33" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>54</v>
       </c>
+      <c r="K35" s="1"/>
       <c r="L35" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>36</v>
       </c>
+      <c r="K36" s="1"/>
       <c r="L36" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>48</v>
       </c>
-      <c r="L38" t="s">
+      <c r="K38" s="1"/>
+      <c r="L38" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>39</v>
       </c>
+      <c r="K42" s="2"/>
       <c r="L42" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>40</v>
       </c>
-      <c r="N45" s="1"/>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K45" s="1"/>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
       <c r="B47" t="s">
         <v>41</v>
       </c>
+      <c r="K47" s="1"/>
       <c r="L47" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>44</v>
       </c>
+      <c r="K51" s="2"/>
       <c r="L51" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>45</v>
       </c>
-      <c r="N52" s="1"/>
-    </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K52" s="1"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>46</v>
       </c>
+      <c r="K53" s="1"/>
       <c r="L53" t="s">
         <v>52</v>
       </c>
@@ -936,6 +974,7 @@
     <mergeCell ref="A3:A7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1130,4 +1169,82 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E2E594-8040-45DC-B516-9788F936830C}">
+  <dimension ref="G11:N12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="11" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>500</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <f>G12*H12</f>
+        <v>1000</v>
+      </c>
+      <c r="J12">
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <f>I12*J12</f>
+        <v>3000</v>
+      </c>
+      <c r="L12">
+        <f>K12/6</f>
+        <v>500</v>
+      </c>
+      <c r="M12">
+        <v>6</v>
+      </c>
+      <c r="N12">
+        <f>L12*M12</f>
+        <v>3000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
observaciones 17 de mayo
observaciones 17 de mayo
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176CCE1B-DB08-452E-BC24-9CC5CD87BE41}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2396445E-ACFD-4FCC-AE5B-091B5861B4FD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprints" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="74">
   <si>
     <t>Observaciones</t>
   </si>
@@ -214,13 +214,49 @@
   </si>
   <si>
     <t>Costo Sesion Total</t>
+  </si>
+  <si>
+    <t>Cuando se van agregando los productos a la tablita se agregan al inicio el que se dio de alta y no al final</t>
+  </si>
+  <si>
+    <t>Hand Held</t>
+  </si>
+  <si>
+    <t>*Bitacoras</t>
+  </si>
+  <si>
+    <t>*Parte de seguimiento</t>
+  </si>
+  <si>
+    <t>Generar notificacion  pediente de atender</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>configuracion de clientes desde administrador</t>
+  </si>
+  <si>
+    <t>Cuando se realice una venta a un cliente tipo merma o tipo saldo requeire firma  del suervisor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Agregar filtro por usuario en ventas y agregar  monto </t>
+  </si>
+  <si>
+    <t>En el reporte de venta agregar si fue pago con tarjeta o efectivo en al reporte de ventas/editar ventas</t>
+  </si>
+  <si>
+    <t>En los pedidos internos cuando son atendidos desde el lado del almacen  en la tienda los debe de ver cualquier usuario de la tienda aunque el no lo haya solicitado</t>
+  </si>
+  <si>
+    <t>Generar notificacion pedido aprobado</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +279,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +318,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -288,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -299,10 +348,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,16 +668,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2A72-8D22-4098-80BD-64C3E85E21F7}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E60" sqref="E60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -649,7 +700,7 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -659,7 +710,7 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -667,7 +718,7 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
+      <c r="A5" s="10"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -675,7 +726,7 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+      <c r="A6" s="10"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -683,7 +734,7 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
+      <c r="A7" s="10"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -691,7 +742,7 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
+      <c r="A8" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -701,7 +752,7 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
+      <c r="A9" s="10"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -709,7 +760,7 @@
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="10"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -839,6 +890,7 @@
         <v>1100</v>
       </c>
     </row>
+    <row r="30" spans="1:13" s="9" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
@@ -855,7 +907,7 @@
       <c r="B32" t="s">
         <v>33</v>
       </c>
-      <c r="K32" s="2"/>
+      <c r="K32" s="1"/>
       <c r="L32" t="s">
         <v>53</v>
       </c>
@@ -898,7 +950,7 @@
         <v>48</v>
       </c>
       <c r="K38" s="1"/>
-      <c r="L38" s="9" t="s">
+      <c r="L38" s="8" t="s">
         <v>47</v>
       </c>
     </row>
@@ -911,7 +963,7 @@
       <c r="B42" t="s">
         <v>39</v>
       </c>
-      <c r="K42" s="2"/>
+      <c r="K42" s="1"/>
       <c r="L42" t="s">
         <v>49</v>
       </c>
@@ -934,7 +986,7 @@
       <c r="B47" t="s">
         <v>41</v>
       </c>
-      <c r="K47" s="1"/>
+      <c r="K47" s="2"/>
       <c r="L47" t="s">
         <v>50</v>
       </c>
@@ -960,12 +1012,72 @@
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="B53" s="8" t="s">
         <v>46</v>
       </c>
       <c r="K53" s="1"/>
       <c r="L53" t="s">
         <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" s="11" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>63</v>
+      </c>
+      <c r="B62" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1175,7 +1287,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E2E594-8040-45DC-B516-9788F936830C}">
   <dimension ref="G11:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
sprint- entrega 28 de mayo
sprint- entrega 28 de mayo
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92FF6E8-2A16-4D22-B818-F75690291E54}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E936BE-2D17-4ABA-9F93-2D360C33F530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
     <sheet name="Hoja4" sheetId="4" r:id="rId4"/>
+    <sheet name="Hoja1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="115">
   <si>
     <t>Observaciones</t>
   </si>
@@ -171,113 +172,215 @@
     <t xml:space="preserve">agregar el cambio de la venta pasada </t>
   </si>
   <si>
+    <t>que se active la alert solo con las ventas en efectivo  dinero fisico</t>
+  </si>
+  <si>
+    <t>Cantidad de Devoluciones por producto o por venta?</t>
+  </si>
+  <si>
+    <t>Cooperacion</t>
+  </si>
+  <si>
+    <t>TotalSesiones</t>
+  </si>
+  <si>
+    <t>Costo Por Hora</t>
+  </si>
+  <si>
+    <t>No.Horas</t>
+  </si>
+  <si>
+    <t>Costo Sesion Por Persona</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Costo Sesion Total</t>
+  </si>
+  <si>
+    <t>Cuando se van agregando los productos a la tablita se agregan al inicio el que se dio de alta y no al final</t>
+  </si>
+  <si>
+    <t>Hand Held</t>
+  </si>
+  <si>
+    <t>*Bitacoras</t>
+  </si>
+  <si>
+    <t>*Parte de seguimiento</t>
+  </si>
+  <si>
+    <t>Generar notificacion  pediente de atender</t>
+  </si>
+  <si>
+    <t>Clientes</t>
+  </si>
+  <si>
+    <t>configuracion de clientes desde administrador</t>
+  </si>
+  <si>
+    <t>En el reporte de venta agregar si fue pago con tarjeta o efectivo en al reporte de ventas/editar ventas</t>
+  </si>
+  <si>
+    <t>En los pedidos internos cuando son atendidos desde el lado del almacen  en la tienda los debe de ver cualquier usuario de la tienda aunque el no lo haya solicitado</t>
+  </si>
+  <si>
+    <t>Generar notificacion pedido aprobado</t>
+  </si>
+  <si>
+    <t>Agregar filtro por usuario en ventas y agregar  monto  y el tipo de pago (efectivo / tarjeta)</t>
+  </si>
+  <si>
+    <t>Cuando se realice una venta a un cliente tipo merma o tipo saldo requeire firma  del supervisor</t>
+  </si>
+  <si>
+    <t>Producto</t>
+  </si>
+  <si>
+    <t>escoba</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Merma</t>
+  </si>
+  <si>
+    <t>Venta Total</t>
+  </si>
+  <si>
+    <t>Saldo</t>
+  </si>
+  <si>
+    <t>consultar ventas en orden ascenden las primeras 50 ya si es con filtro muestra todas</t>
+  </si>
+  <si>
+    <t>Por Revisar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Punto de Venta</t>
+  </si>
+  <si>
+    <t>Agregar el Monto total de la venta al lado de Resumen de la venta en color ROJO u otro y aumentar la fuente</t>
+  </si>
+  <si>
+    <t>Actualizacion Almacenes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Tickets</t>
+  </si>
+  <si>
+    <t>yo como usuario al devolver ticket o agregar generar un nuevo ticket (ticket de devolucion  y complemento) ticket nuevo.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> con la finalidad de identificar  si existe una devolucion o complemento.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Permitir devoluiciones hasta 30 dias (pendiente de definir si es a final de mes o 30 dias naturales.)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5 complementos en el dia.</t>
+  </si>
+  <si>
+    <t>Reportes</t>
+  </si>
+  <si>
+    <t>Inventario -&gt; Tardar mucho</t>
+  </si>
+  <si>
+    <t>Dias promedio de inventario, rango de fechas</t>
+  </si>
+  <si>
+    <t>15 dias</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t>21 dias</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6 productos de mayoreo</t>
+  </si>
+  <si>
+    <t>DashBoard</t>
+  </si>
+  <si>
+    <t>Quitar la ventana de el envase y que se agregue como naturalmente se agregar cualquier producto (quitarla)</t>
+  </si>
+  <si>
+    <t>jessy</t>
+  </si>
+  <si>
     <t>Jessy</t>
   </si>
   <si>
-    <t>que se active la alert solo con las ventas en efectivo  dinero fisico</t>
-  </si>
-  <si>
-    <t>Adrian</t>
-  </si>
-  <si>
-    <t>jessy</t>
-  </si>
-  <si>
     <t>erny</t>
   </si>
   <si>
-    <t>Erni</t>
-  </si>
-  <si>
-    <t>Cantidad de Devoluciones por producto o por venta?</t>
-  </si>
-  <si>
-    <t>Cooperacion</t>
-  </si>
-  <si>
-    <t>TotalSesiones</t>
-  </si>
-  <si>
-    <t>Costo Por Hora</t>
-  </si>
-  <si>
-    <t>No.Horas</t>
-  </si>
-  <si>
-    <t>Costo Sesion Por Persona</t>
-  </si>
-  <si>
-    <t>Personas</t>
-  </si>
-  <si>
-    <t>Costo Sesion Total</t>
-  </si>
-  <si>
-    <t>Cuando se van agregando los productos a la tablita se agregan al inicio el que se dio de alta y no al final</t>
-  </si>
-  <si>
-    <t>Hand Held</t>
-  </si>
-  <si>
-    <t>*Bitacoras</t>
-  </si>
-  <si>
-    <t>*Parte de seguimiento</t>
-  </si>
-  <si>
-    <t>Generar notificacion  pediente de atender</t>
-  </si>
-  <si>
-    <t>Clientes</t>
-  </si>
-  <si>
-    <t>configuracion de clientes desde administrador</t>
-  </si>
-  <si>
-    <t>En el reporte de venta agregar si fue pago con tarjeta o efectivo en al reporte de ventas/editar ventas</t>
-  </si>
-  <si>
-    <t>En los pedidos internos cuando son atendidos desde el lado del almacen  en la tienda los debe de ver cualquier usuario de la tienda aunque el no lo haya solicitado</t>
-  </si>
-  <si>
-    <t>Generar notificacion pedido aprobado</t>
-  </si>
-  <si>
-    <t>Agregar filtro por usuario en ventas y agregar  monto  y el tipo de pago (efectivo / tarjeta)</t>
-  </si>
-  <si>
-    <t>Cuando se realice una venta a un cliente tipo merma o tipo saldo requeire firma  del supervisor</t>
-  </si>
-  <si>
-    <t>Producto</t>
-  </si>
-  <si>
-    <t>escoba</t>
-  </si>
-  <si>
-    <t>Cliente</t>
-  </si>
-  <si>
-    <t>Merma</t>
-  </si>
-  <si>
-    <t>Venta Total</t>
-  </si>
-  <si>
-    <t>Saldo</t>
-  </si>
-  <si>
-    <t>Victor</t>
-  </si>
-  <si>
-    <t>consultar ventas en orden ascenden las primeras 50 ya si es con filtro muestra todas</t>
+    <t xml:space="preserve"> 5 devoluciones</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Generar ticket historial. De complementos o devoluciones</t>
+  </si>
+  <si>
+    <t>padre</t>
+  </si>
+  <si>
+    <t>hijo</t>
+  </si>
+  <si>
+    <t>complemento</t>
+  </si>
+  <si>
+    <t>devolucion</t>
+  </si>
+  <si>
+    <t>IdVenta</t>
+  </si>
+  <si>
+    <t>codigo barras</t>
+  </si>
+  <si>
+    <t>Se debe generar una nueva venta por cada complemento o devolucion o basta con el ticket padre ver el detalle</t>
+  </si>
+  <si>
+    <t>idPadre</t>
+  </si>
+  <si>
+    <t>Proponer que sobre el ticket padre  ver historial tickets visualizar todos los tickets de complemento  y devoluciones</t>
+  </si>
+  <si>
+    <t>Cuando realizo complemento sigue afectando a la cajero que inicio la venta.</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>Asignar a almacen tienda un almacen general para que solo pueda ver productos de jarcieria.</t>
+  </si>
+  <si>
+    <t>Afeca al tipo de usuario  y agregar usuario</t>
+  </si>
+  <si>
+    <t>Agregar tienda liquidos a un almacen liquidos para que solo pueda ver productos de liquidos, en pedidos especiales se surte de la misma tienda.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,8 +410,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -345,6 +470,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -358,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -373,9 +504,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,6 +524,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>417634</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BBCAFC3D-877B-4504-8D4F-CC0C65C5615D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3009900" y="19431000"/>
+          <a:ext cx="6961309" cy="3314700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -690,10 +872,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2A72-8D22-4098-80BD-64C3E85E21F7}">
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="K104" sqref="H104:K104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -701,6 +883,7 @@
     <col min="1" max="1" width="45.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -722,7 +905,7 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -732,7 +915,7 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="12"/>
+      <c r="A4" s="13"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -740,7 +923,7 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="12"/>
+      <c r="A5" s="13"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -748,7 +931,7 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="12"/>
+      <c r="A6" s="13"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -756,7 +939,7 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="12"/>
+      <c r="A7" s="13"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -764,7 +947,7 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -774,7 +957,7 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="12"/>
+      <c r="A9" s="13"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -782,7 +965,7 @@
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
+      <c r="A10" s="13"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -921,60 +1104,43 @@
         <v>32</v>
       </c>
       <c r="K31" s="1"/>
-      <c r="L31" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>33</v>
       </c>
       <c r="K32" s="1"/>
-      <c r="L32" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>34</v>
       </c>
       <c r="K33" s="1"/>
-      <c r="L33" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="K35" s="1"/>
-      <c r="L35" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>36</v>
       </c>
       <c r="K36" s="1"/>
-      <c r="L36" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K38" s="1"/>
-      <c r="L38" s="8" t="s">
-        <v>47</v>
-      </c>
+      <c r="L38" s="8"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -986,9 +1152,6 @@
         <v>39</v>
       </c>
       <c r="K42" s="1"/>
-      <c r="L42" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
@@ -1010,113 +1173,322 @@
       </c>
       <c r="K47" s="2"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>44</v>
       </c>
       <c r="K51" s="1"/>
-      <c r="L51" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>45</v>
       </c>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B53" s="8" t="s">
         <v>46</v>
       </c>
       <c r="K53" s="1"/>
-      <c r="L53" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:11" s="10" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>6</v>
       </c>
       <c r="B56" t="s">
-        <v>71</v>
-      </c>
-      <c r="K56" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="K56" s="1"/>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>61</v>
-      </c>
-      <c r="K57" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="K57" s="1"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>68</v>
-      </c>
-      <c r="K58" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="K59" s="12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>80</v>
-      </c>
-      <c r="K60" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+      <c r="K60" s="1"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="K62" s="1"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="K63" s="1"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>64</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="K64" s="1"/>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="1"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>65</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="K66" s="1"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>70</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="K67" s="1"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K68" s="1"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B70" t="s">
-        <v>67</v>
-      </c>
-      <c r="K70" t="s">
+        <v>62</v>
+      </c>
+      <c r="K70" s="1"/>
+    </row>
+    <row r="72" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>95</v>
+      </c>
+      <c r="J74" t="s">
+        <v>90</v>
+      </c>
+      <c r="K74" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>77</v>
+      </c>
+      <c r="J75" t="s">
+        <v>90</v>
+      </c>
+      <c r="K75" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>84</v>
+      </c>
+      <c r="K76" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>78</v>
+      </c>
+      <c r="B82" t="s">
+        <v>112</v>
+      </c>
+      <c r="J82" t="s">
+        <v>89</v>
+      </c>
+      <c r="K82" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>114</v>
+      </c>
+      <c r="J83" t="s">
+        <v>89</v>
+      </c>
+      <c r="K83" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>113</v>
+      </c>
+      <c r="J84" t="s">
+        <v>89</v>
+      </c>
+      <c r="L84" s="1"/>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>81</v>
+      </c>
+      <c r="J87" t="s">
+        <v>111</v>
+      </c>
+      <c r="K87" t="s">
+        <v>98</v>
+      </c>
+      <c r="L87" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>82</v>
+      </c>
+      <c r="J88" t="s">
+        <v>111</v>
+      </c>
+      <c r="K88" t="s">
+        <v>98</v>
+      </c>
+      <c r="L88" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>100</v>
+      </c>
+      <c r="J89" t="s">
+        <v>111</v>
+      </c>
+      <c r="K89" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>85</v>
+      </c>
+      <c r="J90" t="s">
+        <v>89</v>
+      </c>
+      <c r="K90" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>99</v>
+      </c>
+      <c r="J91" t="s">
+        <v>89</v>
+      </c>
+      <c r="K91" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>93</v>
+      </c>
+      <c r="J92" t="s">
+        <v>89</v>
+      </c>
+      <c r="K92" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94" t="s">
+        <v>110</v>
+      </c>
+      <c r="J94" t="s">
+        <v>111</v>
+      </c>
+      <c r="K94" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>88</v>
+      </c>
+      <c r="J100" t="s">
+        <v>90</v>
+      </c>
+      <c r="K100" t="s">
+        <v>97</v>
+      </c>
+      <c r="L100" s="1"/>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>83</v>
+      </c>
+      <c r="J101" t="s">
+        <v>90</v>
+      </c>
+      <c r="K101" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="J104" t="s">
+        <v>90</v>
+      </c>
+      <c r="K104" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1124,8 +1496,10 @@
     <mergeCell ref="A8:A10"/>
     <mergeCell ref="A3:A7"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1273,18 +1647,18 @@
   <sheetData>
     <row r="8" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I8" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N8" t="s">
         <v>6</v>
       </c>
       <c r="R8" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I9" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="J9">
         <v>10</v>
@@ -1324,12 +1698,12 @@
     </row>
     <row r="12" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I13" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J13" s="11">
         <v>1</v>
@@ -1337,7 +1711,7 @@
     </row>
     <row r="15" spans="9:18" x14ac:dyDescent="0.25">
       <c r="I15" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="J15" s="11">
         <v>0.5</v>
@@ -1350,16 +1724,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1E2E594-8040-45DC-B516-9788F936830C}">
-  <dimension ref="G11:N12"/>
+  <dimension ref="G11:N24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="19.28515625" customWidth="1"/>
     <col min="9" max="9" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.7109375" customWidth="1"/>
     <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
@@ -1367,28 +1742,28 @@
   <sheetData>
     <row r="11" spans="7:14" x14ac:dyDescent="0.25">
       <c r="G11" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="H11" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="J11" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="K11" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="L11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="M11" t="s">
         <v>10</v>
       </c>
       <c r="N11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="7:14" x14ac:dyDescent="0.25">
@@ -1419,6 +1794,166 @@
       <c r="N12">
         <f>L12*M12</f>
         <v>3000</v>
+      </c>
+    </row>
+    <row r="19" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>105</v>
+      </c>
+      <c r="I19" t="s">
+        <v>101</v>
+      </c>
+      <c r="K19" t="s">
+        <v>106</v>
+      </c>
+      <c r="L19" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G21">
+        <v>2</v>
+      </c>
+      <c r="I21" t="s">
+        <v>102</v>
+      </c>
+      <c r="J21" t="s">
+        <v>103</v>
+      </c>
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>3</v>
+      </c>
+      <c r="I22" t="s">
+        <v>102</v>
+      </c>
+      <c r="J22" t="s">
+        <v>104</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="I23" t="s">
+        <v>102</v>
+      </c>
+      <c r="J23" t="s">
+        <v>103</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="7:12" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>5</v>
+      </c>
+      <c r="I24" t="s">
+        <v>102</v>
+      </c>
+      <c r="J24" t="s">
+        <v>103</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBAEE99A-D61B-4F70-B3D3-7B68F6FEC6A1}">
+  <dimension ref="I9:I36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="9" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="17" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I17" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I19" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="23" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I23" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I25" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I26" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I29" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="35" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I36" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Observaciones para separar pedidos de jarcieria a liquidos
Observaciones para separar pedidos de jarcieria a liquidos
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
+++ b/Analisis/SPRINTs/Sprint7.1Observaciones.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3E936BE-2D17-4ABA-9F93-2D360C33F530}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5703CC4-E780-4289-A045-518CF62F4869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{DB616754-FD7A-410B-8F24-D7DCAF5CF756}"/>
   </bookViews>
@@ -505,10 +505,10 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{050C2A72-8D22-4098-80BD-64C3E85E21F7}">
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K104" sqref="H104:K104"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94:K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,7 +905,7 @@
       <c r="M2" s="4"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -915,7 +915,7 @@
       <c r="M3" s="4"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="B4" t="s">
         <v>4</v>
       </c>
@@ -923,7 +923,7 @@
       <c r="M4" s="4"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -931,7 +931,7 @@
       <c r="M5" s="4"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>14</v>
       </c>
@@ -939,7 +939,7 @@
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="14"/>
       <c r="B7" t="s">
         <v>15</v>
       </c>
@@ -947,7 +947,7 @@
       <c r="M7" s="4"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -957,7 +957,7 @@
       <c r="M8" s="4"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" t="s">
         <v>11</v>
       </c>
@@ -965,7 +965,7 @@
       <c r="M9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="M10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1279,7 +1279,7 @@
       </c>
       <c r="K70" s="1"/>
     </row>
-    <row r="72" spans="1:11" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>76</v>

</xml_diff>